<commit_message>
few changes this morning:
</commit_message>
<xml_diff>
--- a/Z Payment Stuff/TimeSheet.xlsx
+++ b/Z Payment Stuff/TimeSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarryBox\Documents\SK_Investair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarryBox\Documents\SK_Investair\Z Payment Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD200865-5DBE-4E4D-A185-275A78EBF276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECFFF68-E9FF-4154-8639-207CE45C7B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCB685F7-FF14-42C6-8964-184920738DDC}"/>
   </bookViews>
@@ -129,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -137,24 +137,21 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,7 +491,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,13 +504,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -528,14 +525,14 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -550,12 +547,12 @@
       <c r="D3" s="6">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -570,12 +567,12 @@
       <c r="D4" s="6">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -590,12 +587,12 @@
       <c r="D5" s="6">
         <v>8</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="E5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -610,12 +607,12 @@
       <c r="D6" s="6">
         <v>8</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="E6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -630,12 +627,12 @@
       <c r="D7" s="6">
         <v>8</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="E7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -650,12 +647,12 @@
       <c r="D8" s="6">
         <v>8</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="E8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -670,12 +667,12 @@
       <c r="D9" s="6">
         <v>8</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="E9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -690,12 +687,12 @@
       <c r="D10" s="6">
         <v>8</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -710,12 +707,12 @@
       <c r="D11" s="6">
         <v>8</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="E11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -730,12 +727,12 @@
       <c r="D12" s="6">
         <v>8</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="E12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -750,12 +747,12 @@
       <c r="D13" s="6">
         <v>8</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="E13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -770,12 +767,12 @@
       <c r="D14" s="6">
         <v>8</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="E14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -790,12 +787,12 @@
       <c r="D15" s="6">
         <v>8</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="E15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -810,12 +807,12 @@
       <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="E16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -830,12 +827,12 @@
       <c r="D17" s="6">
         <v>4.5</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="E17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -850,12 +847,12 @@
       <c r="D18" s="6">
         <v>8</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="E18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -870,170 +867,172 @@
       <c r="D19" s="6">
         <v>8</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="E19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="2">
         <v>45789</v>
       </c>
-      <c r="B20" s="10">
-        <v>0.375</v>
-      </c>
-      <c r="C20" s="10">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D20" s="12">
-        <v>8</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="B20" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="2">
         <v>45792</v>
       </c>
-      <c r="B21" s="10">
-        <v>0.375</v>
-      </c>
-      <c r="C21" s="10">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D21" s="12">
-        <v>8</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="B21" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="2">
         <v>45793</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="7">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="8">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="E22" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="2">
         <v>45799</v>
       </c>
-      <c r="B23" s="10">
-        <v>0.375</v>
-      </c>
-      <c r="C23" s="10">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D23" s="12">
-        <v>8</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="2">
         <v>45800</v>
       </c>
-      <c r="B24" s="10">
-        <v>0.375</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D24" s="12">
-        <v>8</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="B24" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="A25" s="2">
+        <v>45803</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="A26" s="2">
+        <v>45806</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
@@ -1041,11 +1040,16 @@
       </c>
       <c r="D32">
         <f>SUM(D20:D31)</f>
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E6:H6"/>
     <mergeCell ref="E17:H17"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E19:H19"/>
@@ -1061,11 +1065,6 @@
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E11:H11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>